<commit_message>
Update METR model by adding GUI
</commit_message>
<xml_diff>
--- a/metr_paramsnew.xlsx
+++ b/metr_paramsnew.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wb395723\METR Model\METR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1140C1C-7F55-4B54-9520-33FE90177EA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1E49E71-6647-480B-B183-A7F06B4E5D12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{62D246CE-D1E4-4155-BCE2-507AA1B028A6}"/>
   </bookViews>
@@ -612,13 +612,13 @@
     <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -941,7 +941,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B64" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="H2" sqref="H2:H96"/>
+      <selection pane="bottomRight" activeCell="C66" sqref="C66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1069,7 +1069,7 @@
       <c r="G2" t="s">
         <v>70</v>
       </c>
-      <c r="H2" s="30">
+      <c r="H2" s="28">
         <f>IF(G2="FIFO", 1, 0)</f>
         <v>0</v>
       </c>
@@ -1159,7 +1159,7 @@
       <c r="G3" t="s">
         <v>70</v>
       </c>
-      <c r="H3" s="30">
+      <c r="H3" s="28">
         <f t="shared" ref="H3:H66" si="0">IF(G3="FIFO", 1, 0)</f>
         <v>0</v>
       </c>
@@ -1249,7 +1249,7 @@
       <c r="G4" t="s">
         <v>71</v>
       </c>
-      <c r="H4" s="30">
+      <c r="H4" s="28">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1339,7 +1339,7 @@
       <c r="G5" t="s">
         <v>72</v>
       </c>
-      <c r="H5" s="30">
+      <c r="H5" s="28">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -1429,7 +1429,7 @@
       <c r="G6" t="s">
         <v>71</v>
       </c>
-      <c r="H6" s="30">
+      <c r="H6" s="28">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1519,7 +1519,7 @@
       <c r="G7" t="s">
         <v>70</v>
       </c>
-      <c r="H7" s="30">
+      <c r="H7" s="28">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1609,7 +1609,7 @@
       <c r="G8" t="s">
         <v>72</v>
       </c>
-      <c r="H8" s="30">
+      <c r="H8" s="28">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -1699,7 +1699,7 @@
       <c r="G9" t="s">
         <v>71</v>
       </c>
-      <c r="H9" s="30">
+      <c r="H9" s="28">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1789,7 +1789,7 @@
       <c r="G10" t="s">
         <v>72</v>
       </c>
-      <c r="H10" s="30">
+      <c r="H10" s="28">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -1879,7 +1879,7 @@
       <c r="G11" t="s">
         <v>70</v>
       </c>
-      <c r="H11" s="30">
+      <c r="H11" s="28">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1969,7 +1969,7 @@
       <c r="G12" t="s">
         <v>71</v>
       </c>
-      <c r="H12" s="30">
+      <c r="H12" s="28">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -2059,7 +2059,7 @@
       <c r="G13" t="s">
         <v>71</v>
       </c>
-      <c r="H13" s="30">
+      <c r="H13" s="28">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -2149,7 +2149,7 @@
       <c r="G14" t="s">
         <v>70</v>
       </c>
-      <c r="H14" s="30">
+      <c r="H14" s="28">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -2239,7 +2239,7 @@
       <c r="G15" t="s">
         <v>72</v>
       </c>
-      <c r="H15" s="30">
+      <c r="H15" s="28">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -2329,7 +2329,7 @@
       <c r="G16" t="s">
         <v>72</v>
       </c>
-      <c r="H16" s="30">
+      <c r="H16" s="28">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -2419,7 +2419,7 @@
       <c r="G17" t="s">
         <v>70</v>
       </c>
-      <c r="H17" s="30">
+      <c r="H17" s="28">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -2509,7 +2509,7 @@
       <c r="G18" t="s">
         <v>71</v>
       </c>
-      <c r="H18" s="30">
+      <c r="H18" s="28">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -2599,7 +2599,7 @@
       <c r="G19" t="s">
         <v>70</v>
       </c>
-      <c r="H19" s="30">
+      <c r="H19" s="28">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -2689,7 +2689,7 @@
       <c r="G20" t="s">
         <v>71</v>
       </c>
-      <c r="H20" s="30">
+      <c r="H20" s="28">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -2779,7 +2779,7 @@
       <c r="G21" t="s">
         <v>70</v>
       </c>
-      <c r="H21" s="30">
+      <c r="H21" s="28">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -2869,7 +2869,7 @@
       <c r="G22" t="s">
         <v>71</v>
       </c>
-      <c r="H22" s="30">
+      <c r="H22" s="28">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -2959,7 +2959,7 @@
       <c r="G23" t="s">
         <v>70</v>
       </c>
-      <c r="H23" s="30">
+      <c r="H23" s="28">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -3049,7 +3049,7 @@
       <c r="G24" t="s">
         <v>70</v>
       </c>
-      <c r="H24" s="30">
+      <c r="H24" s="28">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -3139,7 +3139,7 @@
       <c r="G25" t="s">
         <v>72</v>
       </c>
-      <c r="H25" s="30">
+      <c r="H25" s="28">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -3229,7 +3229,7 @@
       <c r="G26" t="s">
         <v>71</v>
       </c>
-      <c r="H26" s="30">
+      <c r="H26" s="28">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -3319,7 +3319,7 @@
       <c r="G27" t="s">
         <v>70</v>
       </c>
-      <c r="H27" s="30">
+      <c r="H27" s="28">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -3409,7 +3409,7 @@
       <c r="G28" t="s">
         <v>70</v>
       </c>
-      <c r="H28" s="30">
+      <c r="H28" s="28">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -3499,7 +3499,7 @@
       <c r="G29" t="s">
         <v>70</v>
       </c>
-      <c r="H29" s="30">
+      <c r="H29" s="28">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -3589,7 +3589,7 @@
       <c r="G30" t="s">
         <v>70</v>
       </c>
-      <c r="H30" s="30">
+      <c r="H30" s="28">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -3679,7 +3679,7 @@
       <c r="G31" t="s">
         <v>72</v>
       </c>
-      <c r="H31" s="30">
+      <c r="H31" s="28">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -3769,7 +3769,7 @@
       <c r="G32" t="s">
         <v>71</v>
       </c>
-      <c r="H32" s="30">
+      <c r="H32" s="28">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -3859,7 +3859,7 @@
       <c r="G33" t="s">
         <v>70</v>
       </c>
-      <c r="H33" s="30">
+      <c r="H33" s="28">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -3949,7 +3949,7 @@
       <c r="G34" t="s">
         <v>72</v>
       </c>
-      <c r="H34" s="30">
+      <c r="H34" s="28">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -4039,7 +4039,7 @@
       <c r="G35" t="s">
         <v>70</v>
       </c>
-      <c r="H35" s="30">
+      <c r="H35" s="28">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -4129,7 +4129,7 @@
       <c r="G36" t="s">
         <v>70</v>
       </c>
-      <c r="H36" s="30">
+      <c r="H36" s="28">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -4219,7 +4219,7 @@
       <c r="G37" t="s">
         <v>70</v>
       </c>
-      <c r="H37" s="30">
+      <c r="H37" s="28">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -4309,7 +4309,7 @@
       <c r="G38" t="s">
         <v>70</v>
       </c>
-      <c r="H38" s="30">
+      <c r="H38" s="28">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -4399,7 +4399,7 @@
       <c r="G39" t="s">
         <v>70</v>
       </c>
-      <c r="H39" s="30">
+      <c r="H39" s="28">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -4489,7 +4489,7 @@
       <c r="G40" t="s">
         <v>71</v>
       </c>
-      <c r="H40" s="30">
+      <c r="H40" s="28">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -4579,7 +4579,7 @@
       <c r="G41" t="s">
         <v>70</v>
       </c>
-      <c r="H41" s="30">
+      <c r="H41" s="28">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -4669,7 +4669,7 @@
       <c r="G42" t="s">
         <v>72</v>
       </c>
-      <c r="H42" s="30">
+      <c r="H42" s="28">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -4759,7 +4759,7 @@
       <c r="G43" t="s">
         <v>70</v>
       </c>
-      <c r="H43" s="30">
+      <c r="H43" s="28">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -4849,7 +4849,7 @@
       <c r="G44" t="s">
         <v>70</v>
       </c>
-      <c r="H44" s="30">
+      <c r="H44" s="28">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -4939,7 +4939,7 @@
       <c r="G45" t="s">
         <v>70</v>
       </c>
-      <c r="H45" s="30">
+      <c r="H45" s="28">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -5029,7 +5029,7 @@
       <c r="G46" t="s">
         <v>71</v>
       </c>
-      <c r="H46" s="30">
+      <c r="H46" s="28">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -5119,7 +5119,7 @@
       <c r="G47" t="s">
         <v>71</v>
       </c>
-      <c r="H47" s="30">
+      <c r="H47" s="28">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -5209,7 +5209,7 @@
       <c r="G48" t="s">
         <v>70</v>
       </c>
-      <c r="H48" s="30">
+      <c r="H48" s="28">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -5299,7 +5299,7 @@
       <c r="G49" t="s">
         <v>71</v>
       </c>
-      <c r="H49" s="30">
+      <c r="H49" s="28">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -5389,7 +5389,7 @@
       <c r="G50" t="s">
         <v>71</v>
       </c>
-      <c r="H50" s="30">
+      <c r="H50" s="28">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -5479,7 +5479,7 @@
       <c r="G51" t="s">
         <v>70</v>
       </c>
-      <c r="H51" s="30">
+      <c r="H51" s="28">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -5569,7 +5569,7 @@
       <c r="G52" t="s">
         <v>70</v>
       </c>
-      <c r="H52" s="30">
+      <c r="H52" s="28">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -5659,7 +5659,7 @@
       <c r="G53" t="s">
         <v>72</v>
       </c>
-      <c r="H53" s="30">
+      <c r="H53" s="28">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -5749,7 +5749,7 @@
       <c r="G54" t="s">
         <v>70</v>
       </c>
-      <c r="H54" s="30">
+      <c r="H54" s="28">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -5839,7 +5839,7 @@
       <c r="G55" t="s">
         <v>70</v>
       </c>
-      <c r="H55" s="30">
+      <c r="H55" s="28">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -5929,7 +5929,7 @@
       <c r="G56" t="s">
         <v>70</v>
       </c>
-      <c r="H56" s="30">
+      <c r="H56" s="28">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -6019,7 +6019,7 @@
       <c r="G57" t="s">
         <v>70</v>
       </c>
-      <c r="H57" s="30">
+      <c r="H57" s="28">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -6109,7 +6109,7 @@
       <c r="G58" t="s">
         <v>70</v>
       </c>
-      <c r="H58" s="30">
+      <c r="H58" s="28">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -6199,7 +6199,7 @@
       <c r="G59" t="s">
         <v>70</v>
       </c>
-      <c r="H59" s="30">
+      <c r="H59" s="28">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -6289,7 +6289,7 @@
       <c r="G60" t="s">
         <v>70</v>
       </c>
-      <c r="H60" s="30">
+      <c r="H60" s="28">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -6379,7 +6379,7 @@
       <c r="G61" t="s">
         <v>70</v>
       </c>
-      <c r="H61" s="30">
+      <c r="H61" s="28">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -6469,7 +6469,7 @@
       <c r="G62" t="s">
         <v>70</v>
       </c>
-      <c r="H62" s="30">
+      <c r="H62" s="28">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -6559,7 +6559,7 @@
       <c r="G63" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="H63" s="30">
+      <c r="H63" s="28">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -6649,7 +6649,7 @@
       <c r="G64" t="s">
         <v>70</v>
       </c>
-      <c r="H64" s="30">
+      <c r="H64" s="28">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -6739,7 +6739,7 @@
       <c r="G65" t="s">
         <v>70</v>
       </c>
-      <c r="H65" s="30">
+      <c r="H65" s="28">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -6829,7 +6829,7 @@
       <c r="G66" t="s">
         <v>72</v>
       </c>
-      <c r="H66" s="30">
+      <c r="H66" s="28">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -6919,7 +6919,7 @@
       <c r="G67" t="s">
         <v>70</v>
       </c>
-      <c r="H67" s="30">
+      <c r="H67" s="28">
         <f t="shared" ref="H67:H96" si="1">IF(G67="FIFO", 1, 0)</f>
         <v>0</v>
       </c>
@@ -7009,7 +7009,7 @@
       <c r="G68" t="s">
         <v>72</v>
       </c>
-      <c r="H68" s="30">
+      <c r="H68" s="28">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
@@ -7099,7 +7099,7 @@
       <c r="G69" t="s">
         <v>70</v>
       </c>
-      <c r="H69" s="30">
+      <c r="H69" s="28">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -7189,7 +7189,7 @@
       <c r="G70" t="s">
         <v>72</v>
       </c>
-      <c r="H70" s="30">
+      <c r="H70" s="28">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
@@ -7279,7 +7279,7 @@
       <c r="G71" t="s">
         <v>70</v>
       </c>
-      <c r="H71" s="30">
+      <c r="H71" s="28">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -7369,7 +7369,7 @@
       <c r="G72" t="s">
         <v>72</v>
       </c>
-      <c r="H72" s="30">
+      <c r="H72" s="28">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
@@ -7459,7 +7459,7 @@
       <c r="G73" t="s">
         <v>70</v>
       </c>
-      <c r="H73" s="30">
+      <c r="H73" s="28">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -7549,7 +7549,7 @@
       <c r="G74" t="s">
         <v>71</v>
       </c>
-      <c r="H74" s="30">
+      <c r="H74" s="28">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -7639,7 +7639,7 @@
       <c r="G75" t="s">
         <v>70</v>
       </c>
-      <c r="H75" s="30">
+      <c r="H75" s="28">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -7729,7 +7729,7 @@
       <c r="G76" t="s">
         <v>70</v>
       </c>
-      <c r="H76" s="30">
+      <c r="H76" s="28">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -7819,7 +7819,7 @@
       <c r="G77" t="s">
         <v>70</v>
       </c>
-      <c r="H77" s="30">
+      <c r="H77" s="28">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -7909,7 +7909,7 @@
       <c r="G78" t="s">
         <v>70</v>
       </c>
-      <c r="H78" s="30">
+      <c r="H78" s="28">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -7999,7 +7999,7 @@
       <c r="G79" t="s">
         <v>71</v>
       </c>
-      <c r="H79" s="30">
+      <c r="H79" s="28">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -8089,7 +8089,7 @@
       <c r="G80" t="s">
         <v>70</v>
       </c>
-      <c r="H80" s="30">
+      <c r="H80" s="28">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -8179,7 +8179,7 @@
       <c r="G81" t="s">
         <v>70</v>
       </c>
-      <c r="H81" s="30">
+      <c r="H81" s="28">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -8269,7 +8269,7 @@
       <c r="G82" t="s">
         <v>70</v>
       </c>
-      <c r="H82" s="30">
+      <c r="H82" s="28">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -8359,7 +8359,7 @@
       <c r="G83" t="s">
         <v>70</v>
       </c>
-      <c r="H83" s="30">
+      <c r="H83" s="28">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -8449,7 +8449,7 @@
       <c r="G84" t="s">
         <v>72</v>
       </c>
-      <c r="H84" s="30">
+      <c r="H84" s="28">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
@@ -8539,7 +8539,7 @@
       <c r="G85" t="s">
         <v>70</v>
       </c>
-      <c r="H85" s="30">
+      <c r="H85" s="28">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -8629,7 +8629,7 @@
       <c r="G86" t="s">
         <v>70</v>
       </c>
-      <c r="H86" s="30">
+      <c r="H86" s="28">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -8719,7 +8719,7 @@
       <c r="G87" t="s">
         <v>70</v>
       </c>
-      <c r="H87" s="30">
+      <c r="H87" s="28">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -8809,7 +8809,7 @@
       <c r="G88" t="s">
         <v>70</v>
       </c>
-      <c r="H88" s="30">
+      <c r="H88" s="28">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -8899,7 +8899,7 @@
       <c r="G89" t="s">
         <v>70</v>
       </c>
-      <c r="H89" s="30">
+      <c r="H89" s="28">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -8989,7 +8989,7 @@
       <c r="G90" t="s">
         <v>70</v>
       </c>
-      <c r="H90" s="30">
+      <c r="H90" s="28">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -9079,7 +9079,7 @@
       <c r="G91" t="s">
         <v>70</v>
       </c>
-      <c r="H91" s="30">
+      <c r="H91" s="28">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -9169,7 +9169,7 @@
       <c r="G92" t="s">
         <v>71</v>
       </c>
-      <c r="H92" s="30">
+      <c r="H92" s="28">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -9259,7 +9259,7 @@
       <c r="G93" t="s">
         <v>70</v>
       </c>
-      <c r="H93" s="30">
+      <c r="H93" s="28">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -9349,7 +9349,7 @@
       <c r="G94" t="s">
         <v>71</v>
       </c>
-      <c r="H94" s="30">
+      <c r="H94" s="28">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -9439,7 +9439,7 @@
       <c r="G95" t="s">
         <v>70</v>
       </c>
-      <c r="H95" s="30">
+      <c r="H95" s="28">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -9529,7 +9529,7 @@
       <c r="G96" t="s">
         <v>70</v>
       </c>
-      <c r="H96" s="30">
+      <c r="H96" s="28">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -9628,17 +9628,17 @@
       </c>
     </row>
     <row r="2" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="28" t="s">
+      <c r="B2" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="28"/>
+      <c r="C2" s="29"/>
       <c r="D2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="28" t="s">
+      <c r="E2" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="29"/>
+      <c r="F2" s="30"/>
       <c r="G2" s="5" t="s">
         <v>2</v>
       </c>
@@ -9666,12 +9666,12 @@
       <c r="E3" s="7"/>
       <c r="F3" s="7"/>
       <c r="G3" s="7"/>
-      <c r="H3" s="28" t="s">
+      <c r="H3" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="I3" s="28"/>
-      <c r="J3" s="28"/>
-      <c r="K3" s="28"/>
+      <c r="I3" s="29"/>
+      <c r="J3" s="29"/>
+      <c r="K3" s="29"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">

</xml_diff>